<commit_message>
feat: criação dos casos de teste das User Story US14, US15 e US16
</commit_message>
<xml_diff>
--- a/docs/images/Backlog-e-Casos-Testes-3DSM.xlsx
+++ b/docs/images/Backlog-e-Casos-Testes-3DSM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="230">
   <si>
     <t>Sprint</t>
   </si>
@@ -876,27 +876,117 @@
     <t>CE10.001 - Tela de exibição do gráfico de curva "S"</t>
   </si>
   <si>
-    <t>Dado que eu essteja na tela do gráfico,
-E verifico a existência dos dados da estimativas do cronograma
-e dados do progersso real do  projeto,
+    <t>Dado que eu esteja na tela de acompanhamento,
+E verifico dois eixos no gráfico,
+Eixo mês e ano(Y) e eixo porcentagem(X),
+E verifico a existêcia de duas linhas,
+uma azul e outra vermelha,
+sendo a linha azul para o planejado
+e a linha vermelha para o executado,
 Então válido a exibição da curva "S" no gráfico.</t>
   </si>
   <si>
-    <t>CE10.002 - Progressos do projeto, conforme conclusão de tarefas</t>
+    <t>CE10.002 - Exibição gráfica específica de subníveis do projeto</t>
   </si>
   <si>
-    <t>1 - Deve haver uma tela que exiba um grafico de curva "S", com base no planejamento (cronograma de estimativas) e no progresso real do projeto 
-2 - Na vertical deve haver uma listagem de todos os subníveis do projeto, permitindo a filtragem do grafico, para exibição específica de cada subnível do projeto 
-3 - Na horizontal, deve haver todos os meses estimados da duração do projeto, permitindo a filtragem do grafico, para exibição específica de cada mês do projeto</t>
+    <t>Dado que eu esteja na tela de acompanhamento,
+E visualizo uma lista de subníveis deste projeto na vertical esquerda do gráfico,
+E tendo filtrar um subnível deste projeto,
+Então é exibido um gráfico específico deste subnível filtrado.</t>
   </si>
   <si>
-    <t>CE10.003 - Execução de tarefa</t>
+    <t>CE10.003 - Exibição gráfica dos meses estimados do projeto</t>
   </si>
   <si>
-    <t>CE10.004 - Aumento do progresso proporcional ao peso da tarefa</t>
+    <t>Dado que eu esteja na tela de acompanhamento,
+E visualizo todos os meses de duração estimada do projeto na horizontal superior do gráfico,
+E tendo filtrar um mês deste projeto,
+Então é exibido um gráfico específico deste mês filtrado.</t>
   </si>
   <si>
-    <t>CE10.005 - Persistência do progresso no banco de dados</t>
+    <t>CE11 -
+US15 - Geração de um arquivo excel com o status de avanço em cada subnível do projeto</t>
+  </si>
+  <si>
+    <t>CE11.001 - Botão de gerar arquivo excel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">Dado que eu esteja na </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FFFF0000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>tela...,</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">
+Visualizo o botão de gerar um arquivo excel,
+Então clico no botão e o arquivo é gerado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="&quot;Noto Sans&quot;"/>
+        <color rgb="FF1A1A1A"/>
+      </rPr>
+      <t xml:space="preserve">1 - Deve haver um botão com a opção de gerar um arquivo excel com o status de avanço em cada nível do projeto </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="&quot;Noto Sans&quot;"/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>(*pensar onde vai ficar o botão)</t>
+    </r>
+  </si>
+  <si>
+    <t>CE11.002 - Excel gerado com os dados dos níveis do projeto e progresso de cada nível</t>
+  </si>
+  <si>
+    <t>Dado que eu tenha gerado um arquivo excel,
+E visualizo todos os níveis do projeto na horizontal do arquivo,
+Todos os meses e a porcentagem de avanço de cada nível,
+Então válido que a geração do arquivo foi efetuada corretamente.</t>
+  </si>
+  <si>
+    <t>CE12 -
+US15 - Cadastro de usuário</t>
+  </si>
+  <si>
+    <t>CE15.001 - Tela de cadastro do usuário</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja na tela home de usuários,
+E visualizo um botão escrito "novo",
+E clico nesse botão,
+Então sou direcionado(a) para a tela de cadastro de novo usuário.</t>
+  </si>
+  <si>
+    <t>CE15.002 - Existência dos campos a serem preenchidos com os dados do novo usuário</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja na tela de cadastro de usuário,
+Então visualizo os seguintes campos a serem preenchidos
+"nome completo", "e-mail",
+"cpf", "senha", "confirma senha", "telefone", e "cargo",</t>
+  </si>
+  <si>
+    <t>CE15.003 - Estilização das páginas de usuário</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1379,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1523,6 +1613,10 @@
     <xf borderId="0" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="9" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -21613,101 +21707,135 @@
         <v>214</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="D10" s="64" t="s">
         <v>105</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="47"/>
-      <c r="G10" s="80" t="s">
-        <v>215</v>
-      </c>
+      <c r="G10" s="80"/>
     </row>
     <row r="11">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63" t="s">
+      <c r="A11" s="65"/>
+      <c r="B11" s="71" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="64" t="s">
+      <c r="C11" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="70"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="77"/>
     </row>
     <row r="12">
-      <c r="A12" s="62"/>
+      <c r="A12" s="68" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" s="63" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="D12" s="64" t="s">
         <v>105</v>
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
+      <c r="G12" s="81" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="65"/>
       <c r="B13" s="71" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C13" s="72" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="D13" s="67" t="s">
         <v>105</v>
       </c>
       <c r="E13" s="52"/>
       <c r="F13" s="53"/>
+      <c r="G13" s="82"/>
     </row>
     <row r="14">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="74"/>
+      <c r="A14" s="68" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15">
-      <c r="A15" s="73"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="74"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="79" t="s">
-        <v>210</v>
-      </c>
+      <c r="A16" s="65"/>
+      <c r="B16" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="72"/>
+      <c r="F16" s="77"/>
     </row>
     <row r="17">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="74"/>
+      <c r="B17" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="72"/>
+      <c r="F17" s="77"/>
     </row>
     <row r="18">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="72"/>
+      <c r="F18" s="77"/>
     </row>
     <row r="19">
       <c r="A19" s="73"/>
@@ -29326,10 +29454,13 @@
       <c r="F970" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>